<commit_message>
Production ready: Clean deployment with HTTPS, custom domain, updated docs
</commit_message>
<xml_diff>
--- a/data/excel/student-data.xlsx
+++ b/data/excel/student-data.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,191 +422,218 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>student_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>batch_number</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>batch_start_date</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>batch_end_date</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
         <is>
           <t>sixerclass_id</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>student_name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>batch_number</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>batch_start_date</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>batch_end_date</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>Rahul Sharma</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>AWS-2024-001</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2024-01-15</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2024-04-15</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>SIX001</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Rahul Sharma</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>AWS-2024-001</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2024-01-15</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>2024-04-15</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>Priya Patel</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>AWS-2024-001</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2024-01-15</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2024-04-15</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>SIX002</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Priya Patel</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>AWS-2024-001</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2024-01-15</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>2024-04-15</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>Amit Kumar</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>AWS-2024-001</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2024-01-15</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2024-04-15</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>SIX003</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Amit Kumar</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>AWS-2024-001</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>2024-01-15</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>2024-04-15</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>Neha Gupta</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>AWS-2024-002</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2024-02-01</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2024-05-01</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>SIX004</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Neha Gupta</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>AWS-2024-002</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>2024-02-01</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>2024-05-01</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>Vikram Singh</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>AWS-2024-002</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2024-02-01</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2024-05-01</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
           <t>SIX005</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Vikram Singh</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>AWS-2024-002</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>2024-02-01</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>2024-05-01</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>Anita Desai</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>AWS-2024-002</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2024-02-01</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2024-05-01</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
           <t>SIX006</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Anita Desai</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>AWS-2024-002</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>2024-02-01</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>2024-05-01</t>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Test Student</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>AWS-000</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2026-01-16</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2026-01-16</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>SIX000</t>
         </is>
       </c>
     </row>

</xml_diff>